<commit_message>
updated poplar sex table
</commit_message>
<xml_diff>
--- a/Supplemental_Code/SupTables_Grayson2021.xlsx
+++ b/Supplemental_Code/SupTables_Grayson2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/SexFindR/Supplemental_Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03880614-DA7A-6347-B1CD-368EFA7622D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57370E58-6A18-494A-B9E8-A5F1AD5B5643}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15760" yWindow="6040" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{3158EE9F-058B-0240-9324-5F7A5FD5C8CD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="567">
   <si>
     <t>Fugu</t>
   </si>
@@ -1563,6 +1563,177 @@
   </si>
   <si>
     <t>male_SRR1821254</t>
+  </si>
+  <si>
+    <t>kmerGWAS</t>
+  </si>
+  <si>
+    <t>GEMMA</t>
+  </si>
+  <si>
+    <t>SRR1820075_1.fastq SRR1820075_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820078_1.fastq SRR1820078_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820081_1.fastq SRR1820081_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820090_1.fastq SRR1820090_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820094_1.fastq SRR1820094_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820099_1.fastq SRR1820099_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820100_1.fastq SRR1820100_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820101_1.fastq SRR1820101_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820102_1.fastq SRR1820102_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820103_1.fastq SRR1820103_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820104_1.fastq SRR1820104_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820110_1.fastq SRR1820110_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820119_1.fastq SRR1820119_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821206_1.fastq SRR1821206_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821207_1.fastq SRR1821207_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821208_1.fastq SRR1821208_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821209_1.fastq SRR1821209_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821210_1.fastq SRR1821210_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821212_1.fastq SRR1821212_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821213_1.fastq SRR1821213_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821214_1.fastq SRR1821214_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821215_1.fastq SRR1821215_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821216_1.fastq SRR1821216_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821223_1.fastq SRR1821223_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821225_1.fastq SRR1821225_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821232_1.fastq SRR1821232_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821233_1.fastq SRR1821233_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820107_1.fastq SRR1820107_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820115_1.fastq SRR1820115_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1820117_1.fastq SRR1820117_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821211_1.fastq SRR1821211_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821227_1.fastq SRR1821227_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821228_1.fastq SRR1821228_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821230_1.fastq SRR1821230_1.fastq 1</t>
+  </si>
+  <si>
+    <t>SRR1821237_1.fastq SRR1821237_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821238_1.fastq SRR1821238_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821239_1.fastq SRR1821239_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821240_1.fastq SRR1821240_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821241_1.fastq SRR1821241_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821244_1.fastq SRR1821244_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821245_1.fastq SRR1821245_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821250_1.fastq SRR1821250_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821252_1.fastq SRR1821252_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821253_1.fastq SRR1821253_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821254_1.fastq SRR1821254_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821235_1.fastq SRR1821235_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821236_1.fastq SRR1821236_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821246_1.fastq SRR1821246_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821247_1.fastq SRR1821247_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821248_1.fastq SRR1821248_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821249_1.fastq SRR1821249_1.fastq 2</t>
+  </si>
+  <si>
+    <t>SRR1821251_1.fastq SRR1821251_1.fastq 2</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>coded sex</t>
   </si>
 </sst>
 </file>
@@ -6220,192 +6391,550 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A1728E-DFEB-6649-8063-98CE16F214B5}">
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="E2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="D3" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="E3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="D4" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="E4" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="E5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="D6" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="E6" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="E7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="D8" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="E8" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="D9" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="E9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="D10" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="E10" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="D11" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="E11" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="D12" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="E12" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="D13" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="E13" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="D14" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="E14" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="D15" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="E15" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="D16" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="E16" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="D17" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="E17" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="D18" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="E18" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="D19" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="E19" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="D20" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="E20" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="D21" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="E21" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="D22" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="E22" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="D23" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="E23" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="D24" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="E24" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="D25" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="E25" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="D26" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="E26" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="D27" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="E27" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="D28" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="E28" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="D29" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="E29" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="D30" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="E30" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="D31" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="E31" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="D32" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="E32" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="D33" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="E33" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="D34" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="E34" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="D35" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="E35" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="D36" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="E36" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>509</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="E37" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="E38" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="E39" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D40" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="E40" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D41" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="E41" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D42" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="E42" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="E43" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="E44" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D45" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="E45" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D46" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="E46" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D47" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="E47" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D48" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="E48" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D49" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="E49" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D50" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="E50" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D51" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="E51" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D52" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="E52" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D53" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="E53" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>